<commit_message>
Plots for expanding window analysis
</commit_message>
<xml_diff>
--- a/significance_results/sobol_sensitivity.xlsx
+++ b/significance_results/sobol_sensitivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Documents\climate_detection_time\climate_detection_time\significance_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB26A1F0-7379-4CF6-B7E1-A4B4B9CA2C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AB6CFA-106E-4A9C-8697-BCA3D1AD26ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3309" yWindow="1534" windowWidth="13148" windowHeight="13029" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>ST</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>upstream flood volume</t>
+  </si>
+  <si>
+    <t>upstream flood volume (expanding window)</t>
   </si>
 </sst>
 </file>
@@ -144,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -165,6 +168,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -837,11 +851,124 @@
         <v>9.2127301999999994E-2</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A24" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0.46195437299815001</v>
+      </c>
+      <c r="C24" s="11">
+        <v>7.2956362130250696E-2</v>
+      </c>
+      <c r="D24" s="11">
+        <v>7.3230080890813301E-2</v>
+      </c>
+      <c r="E24" s="11">
+        <v>5.5874693161228998E-2</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0.39823683670617099</v>
+      </c>
+      <c r="H24" s="11">
+        <v>9.9805788403229706E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0.92006013349176397</v>
+      </c>
+      <c r="C25" s="11">
+        <v>6.9350543294679795E-2</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0.482858019483414</v>
+      </c>
+      <c r="E25" s="11">
+        <v>8.8778916823952905E-2</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="11">
+        <v>-3.1187737164214E-2</v>
+      </c>
+      <c r="H25" s="11">
+        <v>6.4632625152124604E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A26" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="11">
+        <v>1.03245220950482E-4</v>
+      </c>
+      <c r="C26" s="11">
+        <v>8.4604850032981197E-5</v>
+      </c>
+      <c r="D26" s="11">
+        <v>-6.7546926718793003E-4</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1.0749293593814999E-3</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="11">
+        <v>2.7659703169208901E-2</v>
+      </c>
+      <c r="H26" s="11">
+        <v>0.110977851242927</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added pre-whitening to article figures
</commit_message>
<xml_diff>
--- a/significance_results/sobol_sensitivity.xlsx
+++ b/significance_results/sobol_sensitivity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Documents\climate_detection_time\climate_detection_time\significance_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AB6CFA-106E-4A9C-8697-BCA3D1AD26ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F08617-EC7E-4B76-9F20-464428621246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="18">
   <si>
     <t>ST</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>upstream flood volume (expanding window)</t>
+  </si>
+  <si>
+    <t>(no pre-whitening)</t>
+  </si>
+  <si>
+    <t>(with pre-whitening)</t>
   </si>
 </sst>
 </file>
@@ -82,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,21 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,10 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -166,18 +187,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,31 +493,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="6" max="6" width="12.69140625" customWidth="1"/>
+    <col min="11" max="11" width="10.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -506,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -533,7 +567,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -560,7 +594,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -587,7 +621,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -597,8 +631,10 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -606,130 +642,285 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="8" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B11" s="5">
         <v>0.29600437600000001</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C11" s="5">
         <v>3.8115577999999997E-2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D11" s="5">
         <v>-9.3990879999999999E-3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E11" s="5">
         <v>5.1660222999999998E-2</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G11" s="5">
         <v>0.26430613800000002</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H11" s="5">
         <v>6.9097927000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.53749362890832897</v>
+      </c>
+      <c r="L11" s="5">
+        <v>4.96032364045444E-2</v>
+      </c>
+      <c r="M11" s="5">
+        <v>8.0367689999999992E-3</v>
+      </c>
+      <c r="N11" s="5">
+        <v>6.3527682000000002E-2</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0.49672428483253001</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>8.6742059675317895E-2</v>
+      </c>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B12" s="5">
         <v>1.009974036</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>7.2365764999999999E-2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12" s="5">
         <v>0.70601029000000004</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <v>8.8393299999999994E-2</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G12" s="5">
         <v>1.8155549E-2</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H12" s="5">
         <v>7.1049068000000007E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.97055671591946102</v>
+      </c>
+      <c r="L12" s="5">
+        <v>9.2277882157395602E-2</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0.39206228999999998</v>
+      </c>
+      <c r="N12" s="5">
+        <v>8.1593476999999998E-2</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P12" s="5">
+        <v>-8.2987022004007895E-3</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>8.2693333038782693E-2</v>
+      </c>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B13" s="5">
         <v>5.1672734999999997E-2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>1.3980846E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D13" s="5">
         <v>-2.6675840000000002E-3</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="5">
         <v>1.7149019000000001E-2</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G13" s="5">
         <v>4.1862666E-2</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H13" s="5">
         <v>0.14237645700000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I13" s="14"/>
+      <c r="J13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.10652969873841101</v>
+      </c>
+      <c r="L13" s="5">
+        <v>2.4223659726771301E-2</v>
+      </c>
+      <c r="M13" s="5">
+        <v>4.2647597000000002E-2</v>
+      </c>
+      <c r="N13" s="5">
+        <v>2.5772494E-2</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="5">
+        <v>2.3168946466166399E-3</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>9.4912616695740096E-2</v>
+      </c>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -738,237 +929,498 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="8" t="s">
+      <c r="I14" s="14"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
+      <c r="I17" s="14"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B18" s="5">
         <v>0.284415429</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C18" s="5">
         <v>3.6099199999999998E-2</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="5">
         <v>4.2843917000000002E-2</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E18" s="5">
         <v>3.7406096999999999E-2</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G18" s="5">
         <v>0.23172789699999999</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H18" s="5">
         <v>6.5367032000000005E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A18" s="4" t="s">
+      <c r="I18" s="14"/>
+      <c r="J18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0.30385594199999999</v>
+      </c>
+      <c r="L18" s="5">
+        <v>3.4626513999999997E-2</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1.3627450000000001E-3</v>
+      </c>
+      <c r="N18" s="5">
+        <v>4.4950726000000003E-2</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18" s="5">
+        <v>0.29742570099999999</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>5.7581611999999997E-2</v>
+      </c>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B19" s="5">
         <v>1.0357465180000001</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <v>6.3911785999999998E-2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D19" s="5">
         <v>0.767442348</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <v>7.8500433999999994E-2</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="5">
         <v>-2.8451838E-2</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H19" s="5">
         <v>5.8638389999999999E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
+      <c r="I19" s="14"/>
+      <c r="J19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="5">
+        <v>1.011847908</v>
+      </c>
+      <c r="L19" s="5">
+        <v>6.5518191000000003E-2</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0.67439900900000005</v>
+      </c>
+      <c r="N19" s="5">
+        <v>8.4019813999999998E-2</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="5">
+        <v>-3.5289289000000001E-2</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>5.3919348999999998E-2</v>
+      </c>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B20" s="5">
         <v>5.6911619999999996E-3</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C20" s="5">
         <v>5.0291049999999999E-3</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D20" s="5">
         <v>2.0848809999999998E-3</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E20" s="5">
         <v>6.9864280000000003E-3</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G20" s="5">
         <v>-5.7369070000000003E-3</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H20" s="5">
         <v>9.2127301999999994E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22" s="9" t="s">
+      <c r="I20" s="14"/>
+      <c r="J20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="5">
+        <v>4.508003E-3</v>
+      </c>
+      <c r="L20" s="5">
+        <v>4.6548359999999999E-3</v>
+      </c>
+      <c r="M20" s="5">
+        <v>-2.5673639999999999E-3</v>
+      </c>
+      <c r="N20" s="5">
+        <v>3.7777919999999999E-3</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="5">
+        <v>1.8463539999999999E-3</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>8.5729537999999994E-2</v>
+      </c>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A23" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24" s="12" t="s">
+      <c r="I24" s="14"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B25" s="9">
         <v>0.46195437299815001</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C25" s="9">
         <v>7.2956362130250696E-2</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D25" s="9">
         <v>7.3230080890813301E-2</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E25" s="9">
         <v>5.5874693161228998E-2</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G25" s="9">
         <v>0.39823683670617099</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H25" s="9">
         <v>9.9805788403229706E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25" s="12" t="s">
+      <c r="I25" s="14"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B26" s="9">
         <v>0.92006013349176397</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C26" s="9">
         <v>6.9350543294679795E-2</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D26" s="9">
         <v>0.482858019483414</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E26" s="9">
         <v>8.8778916823952905E-2</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G26" s="9">
         <v>-3.1187737164214E-2</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H26" s="9">
         <v>6.4632625152124604E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" s="12" t="s">
+      <c r="I26" s="14"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B27" s="9">
         <v>1.03245220950482E-4</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C27" s="9">
         <v>8.4604850032981197E-5</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D27" s="9">
         <v>-6.7546926718793003E-4</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E27" s="9">
         <v>1.0749293593814999E-3</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G27" s="9">
         <v>2.7659703169208901E-2</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H27" s="9">
         <v>0.110977851242927</v>
       </c>
+      <c r="I27" s="14"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A8:H8"/>
+  <mergeCells count="7">
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="J9:Q9"/>
+    <mergeCell ref="J16:Q16"/>
+    <mergeCell ref="J23:Q23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More updates after prewhitening
</commit_message>
<xml_diff>
--- a/significance_results/sobol_sensitivity.xlsx
+++ b/significance_results/sobol_sensitivity.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Documents\climate_detection_time\climate_detection_time\significance_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F08617-EC7E-4B76-9F20-464428621246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6819AB-DC62-4A91-8955-60887311243B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="8820" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="22">
   <si>
     <t>ST</t>
   </si>
@@ -79,6 +90,18 @@
   </si>
   <si>
     <t>(with pre-whitening)</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>ST - total order sensitivity</t>
+  </si>
+  <si>
+    <t>S1 - first order sensitivity</t>
+  </si>
+  <si>
+    <t>S2 - second order (interaction) sensitivity</t>
   </si>
 </sst>
 </file>
@@ -168,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -195,16 +218,7 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -213,6 +227,18 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,32 +519,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="6" max="6" width="12.69140625" customWidth="1"/>
     <col min="11" max="11" width="10.61328125" customWidth="1"/>
+    <col min="18" max="18" width="7.69140625" customWidth="1"/>
+    <col min="21" max="21" width="9.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -540,7 +568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -567,7 +595,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -594,7 +622,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -621,7 +649,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -631,7 +659,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -642,23 +670,25 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
+      <c r="I7" s="12"/>
+      <c r="J7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -667,48 +697,54 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="12" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="12"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>0</v>
@@ -729,7 +765,7 @@
       <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="3"/>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -750,12 +786,16 @@
       <c r="Q10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R10" s="12"/>
+      <c r="S10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="12"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -780,7 +820,7 @@
       <c r="H11" s="5">
         <v>6.9097927000000003E-2</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="4" t="s">
         <v>4</v>
       </c>
@@ -805,12 +845,16 @@
       <c r="Q11" s="5">
         <v>8.6742059675317895E-2</v>
       </c>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R11" s="12"/>
+      <c r="S11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="12"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -835,7 +879,7 @@
       <c r="H12" s="5">
         <v>7.1049068000000007E-2</v>
       </c>
-      <c r="I12" s="14"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="4" t="s">
         <v>5</v>
       </c>
@@ -860,12 +904,16 @@
       <c r="Q12" s="5">
         <v>8.2693333038782693E-2</v>
       </c>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R12" s="12"/>
+      <c r="S12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="12"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -890,7 +938,7 @@
       <c r="H13" s="5">
         <v>0.14237645700000001</v>
       </c>
-      <c r="I13" s="14"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="4" t="s">
         <v>6</v>
       </c>
@@ -915,12 +963,14 @@
       <c r="Q13" s="5">
         <v>9.4912616695740096E-2</v>
       </c>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -929,7 +979,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="14"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -938,12 +988,14 @@
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -952,7 +1004,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="14"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -961,39 +1013,43 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A16" s="12" t="s">
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="12" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="12"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
         <v>0</v>
@@ -1014,7 +1070,7 @@
       <c r="H17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="14"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="3"/>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1035,12 +1091,14 @@
       <c r="Q17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1123,7 @@
       <c r="H18" s="5">
         <v>6.5367032000000005E-2</v>
       </c>
-      <c r="I18" s="14"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1090,12 +1148,14 @@
       <c r="Q18" s="5">
         <v>5.7581611999999997E-2</v>
       </c>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1120,7 +1180,7 @@
       <c r="H19" s="5">
         <v>5.8638389999999999E-2</v>
       </c>
-      <c r="I19" s="14"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1145,12 +1205,14 @@
       <c r="Q19" s="5">
         <v>5.3919348999999998E-2</v>
       </c>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1175,7 +1237,7 @@
       <c r="H20" s="5">
         <v>9.2127301999999994E-2</v>
       </c>
-      <c r="I20" s="14"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1200,67 +1262,75 @@
       <c r="Q20" s="5">
         <v>8.5729537999999994E-2</v>
       </c>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A23" s="13" t="s">
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A23" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A24" s="8"/>
       <c r="B24" s="8" t="s">
         <v>0</v>
@@ -1281,21 +1351,23 @@
       <c r="H24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="I24" s="12"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>4</v>
       </c>
@@ -1320,21 +1392,22 @@
       <c r="H25" s="9">
         <v>9.9805788403229706E-2</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="I25" s="12"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="W25" s="12"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
         <v>5</v>
       </c>
@@ -1359,21 +1432,21 @@
       <c r="H26" s="9">
         <v>6.4632625152124604E-2</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="I26" s="12"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>6</v>
       </c>
@@ -1398,19 +1471,19 @@
       <c r="H27" s="9">
         <v>0.110977851242927</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1423,5 +1496,6 @@
     <mergeCell ref="J23:Q23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>